<commit_message>
Update Modules based on other projects
</commit_message>
<xml_diff>
--- a/BugList.xlsx
+++ b/BugList.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>PENGATURAN SISTEM APLIKASI</t>
   </si>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t>ERROR DATE TIME FORMAT FOR WINDOWS 10</t>
+  </si>
+  <si>
+    <t>ERROR SALES ORDER REVISION</t>
+  </si>
+  <si>
+    <t>ERROR GENERATE DO LANGSUNG SETELAH PEMBUATAN SO</t>
   </si>
 </sst>
 </file>
@@ -429,8 +435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,6 +510,16 @@
         <v>12</v>
       </c>
     </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>25</v>
+      </c>
+    </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>13</v>

</xml_diff>